<commit_message>
Diagram changed and dimensional model according to etl
</commit_message>
<xml_diff>
--- a/docs/Planning.xlsx
+++ b/docs/Planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\OneDrive\Desktop\AID\FEUP-AID\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED474C6-4435-419F-B51C-1D92EC2AA6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42DDD78-A6D9-43E5-8812-28E400F865EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{4021D660-8C1E-49EA-8FA2-A02854DF6B2D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{4021D660-8C1E-49EA-8FA2-A02854DF6B2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Dimensions" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="203">
   <si>
     <t>Star</t>
   </si>
@@ -301,12 +301,6 @@
     <t>Surrogate key of the rate code.</t>
   </si>
   <si>
-    <t>RateCodeIDOrig</t>
-  </si>
-  <si>
-    <t>Original numeric code from TLC.</t>
-  </si>
-  <si>
     <t>RateCodeDesc</t>
   </si>
   <si>
@@ -325,12 +319,6 @@
     <t>Surrogate key of the payment type.</t>
   </si>
   <si>
-    <t>PaymentTypeCodeOrig</t>
-  </si>
-  <si>
-    <t>Original numeric payment type code.</t>
-  </si>
-  <si>
     <t>PaymentTypeDesc</t>
   </si>
   <si>
@@ -385,9 +373,6 @@
     <t>Surrogate key of the trip characteristics.</t>
   </si>
   <si>
-    <t>StoreAndForwardFlag</t>
-  </si>
-  <si>
     <t>Store-and-forward flag from TLC (Y/N).</t>
   </si>
   <si>
@@ -505,9 +490,6 @@
     <t>PickupLocation / DropoffLocation (role-playing)</t>
   </si>
   <si>
-    <t>TripID</t>
-  </si>
-  <si>
     <t>Dimension</t>
   </si>
   <si>
@@ -658,10 +640,13 @@
     <t>Derived flag (Y/N) if CBD fee or CBD zone.</t>
   </si>
   <si>
-    <t>Identifier from the source dataset  to represent zones</t>
-  </si>
-  <si>
     <t>FactTripKey</t>
+  </si>
+  <si>
+    <t>Identifier to represent zones</t>
+  </si>
+  <si>
+    <t>StoreAndForwardBool</t>
   </si>
 </sst>
 </file>
@@ -1025,7 +1010,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1141,157 +1126,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1304,14 +1151,119 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1646,10 +1598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC0CEAC-D105-4885-94C2-26BF4683722C}">
-  <dimension ref="A1:L94"/>
+  <dimension ref="A1:L89"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1700,9 +1652,8 @@
         <v>3</v>
       </c>
       <c r="G6" s="11">
-        <v>45993</v>
-      </c>
-      <c r="I6" s="94"/>
+        <v>46024</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
@@ -1717,11 +1668,11 @@
       <c r="D7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="43"/>
-      <c r="G7" s="44"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="56"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
@@ -1846,10 +1797,10 @@
         <v>15</v>
       </c>
       <c r="G13" s="15"/>
-      <c r="I13" s="99"/>
-      <c r="J13" s="99"/>
-      <c r="K13" s="99"/>
-      <c r="L13" s="99"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="51"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
@@ -1871,10 +1822,10 @@
       <c r="G14" s="15">
         <v>0</v>
       </c>
-      <c r="I14" s="99"/>
-      <c r="J14" s="99"/>
-      <c r="K14" s="99"/>
-      <c r="L14" s="99"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="51"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
@@ -1896,10 +1847,10 @@
       <c r="G15" s="15">
         <v>0</v>
       </c>
-      <c r="I15" s="99"/>
-      <c r="J15" s="99"/>
-      <c r="K15" s="99"/>
-      <c r="L15" s="99"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="51"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
@@ -1921,10 +1872,10 @@
       <c r="G16" s="15">
         <v>0</v>
       </c>
-      <c r="I16" s="99"/>
-      <c r="J16" s="99"/>
-      <c r="K16" s="99"/>
-      <c r="L16" s="99"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="51"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
@@ -1944,10 +1895,10 @@
         <v>10</v>
       </c>
       <c r="G17" s="15"/>
-      <c r="I17" s="99"/>
-      <c r="J17" s="99"/>
-      <c r="K17" s="99"/>
-      <c r="L17" s="99"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="51"/>
     </row>
     <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
@@ -1961,16 +1912,16 @@
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="18" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="F18" s="18">
         <v>1</v>
       </c>
       <c r="G18" s="19"/>
-      <c r="I18" s="99"/>
-      <c r="J18" s="99"/>
-      <c r="K18" s="99"/>
-      <c r="L18" s="99"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="51"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="42"/>
@@ -1980,14 +1931,14 @@
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
       <c r="G19" s="42"/>
-      <c r="I19" s="99"/>
-      <c r="J19" s="99"/>
-      <c r="K19" s="99"/>
-      <c r="L19" s="99"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
     </row>
     <row r="22" spans="1:12" ht="22.8" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -2010,7 +1961,7 @@
         <v>3</v>
       </c>
       <c r="G23" s="11">
-        <v>45993</v>
+        <v>46024</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -2026,11 +1977,11 @@
       <c r="D24" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="43" t="s">
+      <c r="E24" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="F24" s="43"/>
-      <c r="G24" s="44"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="56"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
@@ -2098,9 +2049,9 @@
       <c r="G27" s="15">
         <v>0</v>
       </c>
-      <c r="I27" s="99"/>
-      <c r="J27" s="99"/>
-      <c r="K27" s="99"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="51"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="16" t="s">
@@ -2122,16 +2073,16 @@
       <c r="G28" s="15">
         <v>0</v>
       </c>
-      <c r="I28" s="99"/>
-      <c r="J28" s="99"/>
-      <c r="K28" s="99"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="51"/>
+      <c r="K28" s="51"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
         <v>57</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>48</v>
@@ -2144,9 +2095,9 @@
         <v>20</v>
       </c>
       <c r="G29" s="15"/>
-      <c r="I29" s="99"/>
-      <c r="J29" s="99"/>
-      <c r="K29" s="99"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="51"/>
     </row>
     <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="17" t="s">
@@ -2166,13 +2117,13 @@
         <v>20</v>
       </c>
       <c r="G30" s="19"/>
-      <c r="I30" s="99"/>
-      <c r="J30" s="99"/>
-      <c r="K30" s="99"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
+      <c r="K30" s="51"/>
     </row>
     <row r="32" spans="1:12" ht="22.8" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A32" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -2195,7 +2146,7 @@
         <v>3</v>
       </c>
       <c r="G33" s="11">
-        <v>45993</v>
+        <v>46024</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2211,11 +2162,11 @@
       <c r="D34" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E34" s="43" t="s">
+      <c r="E34" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="F34" s="43"/>
-      <c r="G34" s="44"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="56"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
@@ -2241,7 +2192,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="89" t="s">
+      <c r="A36" s="16" t="s">
         <v>60</v>
       </c>
       <c r="B36" s="13" t="s">
@@ -2258,11 +2209,11 @@
       </c>
       <c r="F36" s="13"/>
       <c r="G36" s="15"/>
-      <c r="I36" s="99"/>
-      <c r="J36" s="99"/>
+      <c r="I36" s="51"/>
+      <c r="J36" s="51"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="89" t="s">
+      <c r="A37" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B37" s="13" t="s">
@@ -2283,8 +2234,8 @@
       <c r="G37" s="15">
         <v>0</v>
       </c>
-      <c r="I37" s="99"/>
-      <c r="J37" s="99"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="51"/>
     </row>
     <row r="38" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="17" t="s">
@@ -2304,12 +2255,12 @@
         <v>100</v>
       </c>
       <c r="G38" s="19"/>
-      <c r="I38" s="99"/>
-      <c r="J38" s="99"/>
+      <c r="I38" s="51"/>
+      <c r="J38" s="51"/>
     </row>
     <row r="42" spans="1:10" ht="22.8" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A42" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
@@ -2332,7 +2283,7 @@
         <v>3</v>
       </c>
       <c r="G43" s="11">
-        <v>45993</v>
+        <v>46024</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2348,11 +2299,11 @@
       <c r="D44" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E44" s="43" t="s">
+      <c r="E44" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="F44" s="43"/>
-      <c r="G44" s="44"/>
+      <c r="F44" s="55"/>
+      <c r="G44" s="56"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="20" t="s">
@@ -2397,25 +2348,25 @@
       <c r="G46" s="15"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" s="102" t="s">
-        <v>204</v>
-      </c>
-      <c r="B47" s="101" t="s">
-        <v>206</v>
-      </c>
-      <c r="C47" s="101" t="s">
+      <c r="A47" s="53" t="s">
+        <v>198</v>
+      </c>
+      <c r="B47" s="52" t="s">
+        <v>201</v>
+      </c>
+      <c r="C47" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="D47" s="101" t="s">
+      <c r="D47" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="E47" s="101" t="s">
+      <c r="E47" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F47" s="101">
+      <c r="F47" s="52">
         <v>4</v>
       </c>
-      <c r="G47" s="103">
+      <c r="G47" s="54">
         <v>0</v>
       </c>
     </row>
@@ -2488,7 +2439,7 @@
       </c>
       <c r="D51" s="13"/>
       <c r="E51" s="13" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="F51" s="13"/>
       <c r="G51" s="15"/>
@@ -2505,14 +2456,14 @@
       </c>
       <c r="D52" s="18"/>
       <c r="E52" s="18" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="F52" s="18"/>
       <c r="G52" s="19"/>
     </row>
     <row r="54" spans="1:10" ht="22.8" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A54" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
@@ -2535,7 +2486,7 @@
         <v>3</v>
       </c>
       <c r="G55" s="11">
-        <v>45993</v>
+        <v>46024</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2579,11 +2530,11 @@
       <c r="G57" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="I57" s="99"/>
-      <c r="J57" s="99"/>
+      <c r="I57" s="51"/>
+      <c r="J57" s="51"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A58" s="89" t="s">
+      <c r="A58" s="16" t="s">
         <v>85</v>
       </c>
       <c r="B58" s="13" t="s">
@@ -2600,56 +2551,33 @@
       </c>
       <c r="F58" s="13"/>
       <c r="G58" s="15"/>
-      <c r="I58" s="99"/>
-      <c r="J58" s="99"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A59" s="89" t="s">
+      <c r="I58" s="51"/>
+      <c r="J58" s="51"/>
+    </row>
+    <row r="59" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="B59" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C59" s="13" t="s">
+      <c r="C59" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D59" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E59" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F59" s="13">
-        <v>2</v>
-      </c>
-      <c r="G59" s="15">
-        <v>0</v>
-      </c>
-      <c r="I59" s="99"/>
-      <c r="J59" s="99"/>
-    </row>
-    <row r="60" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B60" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="C60" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="D60" s="18"/>
-      <c r="E60" s="18" t="s">
+      <c r="D59" s="18"/>
+      <c r="E59" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F60" s="18">
+      <c r="F59" s="18">
         <v>50</v>
       </c>
-      <c r="G60" s="19"/>
+      <c r="G59" s="19"/>
+      <c r="I59" s="51"/>
+      <c r="J59" s="51"/>
     </row>
     <row r="62" spans="1:10" ht="22.8" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A62" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
@@ -2672,15 +2600,15 @@
         <v>3</v>
       </c>
       <c r="G63" s="11">
-        <v>45993</v>
+        <v>46024</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C64" s="13" t="s">
         <v>11</v>
@@ -2688,13 +2616,13 @@
       <c r="D64" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E64" s="43" t="s">
-        <v>91</v>
-      </c>
-      <c r="F64" s="43"/>
-      <c r="G64" s="44"/>
-      <c r="I64" s="99"/>
-      <c r="J64" s="99"/>
+      <c r="E64" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="F64" s="55"/>
+      <c r="G64" s="56"/>
+      <c r="I64" s="51"/>
+      <c r="J64" s="51"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="20" t="s">
@@ -2718,18 +2646,18 @@
       <c r="G65" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="I65" s="99"/>
-      <c r="J65" s="99"/>
+      <c r="I65" s="51"/>
+      <c r="J65" s="51"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A66" s="89" t="s">
-        <v>93</v>
+      <c r="A66" s="16" t="s">
+        <v>91</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D66" s="13" t="s">
         <v>19</v>
@@ -2739,66 +2667,34 @@
       </c>
       <c r="F66" s="13"/>
       <c r="G66" s="15"/>
-      <c r="I66" s="99"/>
-      <c r="J66" s="99"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A67" s="89" t="s">
-        <v>95</v>
-      </c>
-      <c r="B67" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="C67" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="D67" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E67" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F67" s="13">
-        <v>2</v>
-      </c>
-      <c r="G67" s="15">
-        <v>0</v>
-      </c>
-      <c r="I67" s="99"/>
-      <c r="J67" s="99"/>
-    </row>
-    <row r="68" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="B68" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="C68" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="D68" s="18"/>
-      <c r="E68" s="18" t="s">
+      <c r="I66" s="51"/>
+      <c r="J66" s="51"/>
+    </row>
+    <row r="67" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B67" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F68" s="18">
-        <v>30</v>
-      </c>
-      <c r="G68" s="19"/>
+      <c r="F67" s="18">
+        <v>60</v>
+      </c>
+      <c r="G67" s="19"/>
+      <c r="I67" s="51"/>
+      <c r="J67" s="51"/>
     </row>
     <row r="70" spans="1:10" ht="22.8" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A70" s="80" t="s">
-        <v>126</v>
-      </c>
-      <c r="B70" s="81"/>
-      <c r="C70" s="81"/>
-      <c r="D70" s="81"/>
-      <c r="E70" s="81"/>
-      <c r="F70" s="81"/>
-      <c r="G70" s="81"/>
-      <c r="H70" s="81"/>
-      <c r="I70" s="81"/>
-      <c r="J70" s="81"/>
+      <c r="A70" s="3" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
@@ -2813,40 +2709,34 @@
       <c r="D71" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E71" s="82" t="s">
+      <c r="E71" s="10" t="s">
         <v>2</v>
       </c>
       <c r="F71" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G71" s="83">
-        <v>45993</v>
-      </c>
-      <c r="H71" s="81"/>
-      <c r="I71" s="81"/>
-      <c r="J71" s="81"/>
-    </row>
-    <row r="72" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A72" s="84" t="s">
-        <v>100</v>
-      </c>
-      <c r="B72" s="85" t="s">
-        <v>99</v>
-      </c>
-      <c r="C72" s="85" t="s">
+      <c r="G71" s="11">
+        <v>46024</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A72" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C72" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D72" s="86" t="s">
+      <c r="D72" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E72" s="87" t="s">
-        <v>100</v>
-      </c>
-      <c r="F72" s="87"/>
-      <c r="G72" s="88"/>
-      <c r="H72" s="81"/>
-      <c r="I72" s="81"/>
-      <c r="J72" s="81"/>
+      <c r="E72" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="F72" s="55"/>
+      <c r="G72" s="56"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="20" t="s">
@@ -2870,129 +2760,121 @@
       <c r="G73" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H73" s="81"/>
-      <c r="I73" s="81"/>
-      <c r="J73" s="81"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A74" s="89" t="s">
+      <c r="A74" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C74" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D74" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E74" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F74" s="13"/>
+      <c r="G74" s="15"/>
+      <c r="I74" s="51"/>
+      <c r="J74" s="51"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A75" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B75" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C75" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D75" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F75" s="13">
+        <v>10</v>
+      </c>
+      <c r="G75" s="15"/>
+      <c r="I75" s="51"/>
+      <c r="J75" s="51"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="B74" s="85" t="s">
+      <c r="B76" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="C74" s="85" t="s">
-        <v>100</v>
-      </c>
-      <c r="D74" s="85" t="s">
-        <v>19</v>
-      </c>
-      <c r="E74" s="85" t="s">
-        <v>20</v>
-      </c>
-      <c r="F74" s="85"/>
-      <c r="G74" s="90"/>
-      <c r="H74" s="81"/>
-      <c r="I74" s="100"/>
-      <c r="J74" s="100"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A75" s="89" t="s">
+      <c r="C76" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F76" s="13">
+        <v>50</v>
+      </c>
+      <c r="G76" s="15"/>
+      <c r="I76" s="51"/>
+      <c r="J76" s="51"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="B75" s="85" t="s">
+      <c r="B77" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="C75" s="85" t="s">
-        <v>100</v>
-      </c>
-      <c r="D75" s="85" t="s">
-        <v>21</v>
-      </c>
-      <c r="E75" s="85" t="s">
-        <v>22</v>
-      </c>
-      <c r="F75" s="85">
-        <v>10</v>
-      </c>
-      <c r="G75" s="90"/>
-      <c r="H75" s="81"/>
-      <c r="I75" s="100"/>
-      <c r="J75" s="100"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A76" s="89" t="s">
+      <c r="C77" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F77" s="13">
+        <v>2</v>
+      </c>
+      <c r="G77" s="15">
+        <v>0</v>
+      </c>
+      <c r="I77" s="51"/>
+      <c r="J77" s="51"/>
+    </row>
+    <row r="78" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="B76" s="85" t="s">
+      <c r="B78" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C76" s="85" t="s">
-        <v>100</v>
-      </c>
-      <c r="D76" s="85"/>
-      <c r="E76" s="85" t="s">
-        <v>22</v>
-      </c>
-      <c r="F76" s="85">
-        <v>50</v>
-      </c>
-      <c r="G76" s="90"/>
-      <c r="H76" s="81"/>
-      <c r="I76" s="100"/>
-      <c r="J76" s="100"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A77" s="89" t="s">
-        <v>107</v>
-      </c>
-      <c r="B77" s="85" t="s">
-        <v>108</v>
-      </c>
-      <c r="C77" s="85" t="s">
-        <v>100</v>
-      </c>
-      <c r="D77" s="85"/>
-      <c r="E77" s="85" t="s">
+      <c r="C78" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D78" s="18"/>
+      <c r="E78" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F77" s="85">
+      <c r="F78" s="18">
         <v>2</v>
       </c>
-      <c r="G77" s="90">
+      <c r="G78" s="19">
         <v>0</v>
       </c>
-      <c r="H77" s="81"/>
-      <c r="I77" s="100"/>
-      <c r="J77" s="100"/>
-    </row>
-    <row r="78" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="91" t="s">
-        <v>109</v>
-      </c>
-      <c r="B78" s="92" t="s">
-        <v>110</v>
-      </c>
-      <c r="C78" s="92" t="s">
-        <v>100</v>
-      </c>
-      <c r="D78" s="92"/>
-      <c r="E78" s="92" t="s">
-        <v>30</v>
-      </c>
-      <c r="F78" s="92">
-        <v>2</v>
-      </c>
-      <c r="G78" s="93">
-        <v>0</v>
-      </c>
-      <c r="H78" s="81"/>
-      <c r="I78" s="100"/>
-      <c r="J78" s="100"/>
+      <c r="I78" s="51"/>
+      <c r="J78" s="51"/>
     </row>
     <row r="80" spans="1:10" ht="22.8" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A80" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
@@ -3015,15 +2897,15 @@
         <v>3</v>
       </c>
       <c r="G81" s="11">
-        <v>45993</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>46024</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C82" s="13" t="s">
         <v>25</v>
@@ -3031,11 +2913,11 @@
       <c r="D82" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E82" s="43" t="s">
-        <v>111</v>
-      </c>
-      <c r="F82" s="43"/>
-      <c r="G82" s="44"/>
+      <c r="E82" s="55" t="s">
+        <v>107</v>
+      </c>
+      <c r="F82" s="55"/>
+      <c r="G82" s="56"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" s="20" t="s">
@@ -3062,13 +2944,13 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D84" s="13" t="s">
         <v>19</v>
@@ -3081,102 +2963,100 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" s="16" t="s">
-        <v>115</v>
+        <v>202</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D85" s="13"/>
       <c r="E85" s="13" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="F85" s="13"/>
       <c r="G85" s="15"/>
-      <c r="I85" s="99"/>
-      <c r="J85" s="99"/>
-    </row>
-    <row r="86" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I85" s="51"/>
+      <c r="J85" s="51"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" s="16" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D86" s="13"/>
       <c r="E86" s="13" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="F86" s="13"/>
       <c r="G86" s="15"/>
-      <c r="I86" s="99"/>
-      <c r="J86" s="99"/>
-    </row>
-    <row r="87" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I86" s="51"/>
+      <c r="J86" s="51"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" s="16" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C87" s="13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D87" s="13"/>
       <c r="E87" s="13" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="F87" s="13"/>
       <c r="G87" s="15"/>
-      <c r="I87" s="99"/>
-      <c r="J87" s="99"/>
+      <c r="I87" s="51"/>
+      <c r="J87" s="51"/>
     </row>
     <row r="88" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="17" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B88" s="18" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C88" s="18" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D88" s="18"/>
       <c r="E88" s="18" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="F88" s="18"/>
       <c r="G88" s="19"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A89" s="95"/>
-      <c r="B89" s="95"/>
-      <c r="C89" s="95"/>
-      <c r="D89" s="95"/>
-      <c r="E89" s="95"/>
-      <c r="F89" s="95"/>
-      <c r="G89" s="95"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B94" s="94"/>
+      <c r="A89" s="42"/>
+      <c r="B89" s="42"/>
+      <c r="C89" s="42"/>
+      <c r="D89" s="42"/>
+      <c r="E89" s="42"/>
+      <c r="F89" s="42"/>
+      <c r="G89" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="E82:G82"/>
+    <mergeCell ref="E64:G64"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="E24:G24"/>
     <mergeCell ref="E34:G34"/>
     <mergeCell ref="E44:G44"/>
     <mergeCell ref="E72:G72"/>
-    <mergeCell ref="E82:G82"/>
-    <mergeCell ref="E64:G64"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3185,7 +3065,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3200,19 +3080,19 @@
     </row>
     <row r="2" spans="1:11" ht="22.2" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="97.2" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B4" s="32" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D4" s="34" t="s">
         <v>3</v>
@@ -3230,72 +3110,72 @@
         <v>83</v>
       </c>
       <c r="I4" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="J4" s="96" t="s">
-        <v>111</v>
+        <v>89</v>
+      </c>
+      <c r="J4" s="48" t="s">
+        <v>107</v>
       </c>
       <c r="K4" s="35" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
-        <v>178</v>
-      </c>
-      <c r="B5" s="45" t="s">
-        <v>129</v>
-      </c>
-      <c r="C5" s="45"/>
+        <v>172</v>
+      </c>
+      <c r="B5" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="57"/>
       <c r="D5" s="37" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="G5" s="37" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="H5" s="37" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="I5" s="37" t="s">
-        <v>179</v>
-      </c>
-      <c r="J5" s="97" t="s">
-        <v>179</v>
+        <v>173</v>
+      </c>
+      <c r="J5" s="49" t="s">
+        <v>173</v>
       </c>
       <c r="K5" s="38" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="39"/>
-      <c r="B6" s="46" t="s">
-        <v>159</v>
-      </c>
-      <c r="C6" s="46"/>
+      <c r="B6" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="58"/>
       <c r="D6" s="40" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E6" s="40"/>
       <c r="F6" s="40" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="G6" s="40" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="H6" s="40"/>
       <c r="I6" s="40"/>
-      <c r="J6" s="98"/>
+      <c r="J6" s="50"/>
       <c r="K6" s="41"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
       <c r="D7" s="30"/>
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
@@ -3305,8 +3185,8 @@
       <c r="J7" s="30"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
@@ -3316,8 +3196,8 @@
       <c r="J8" s="30"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
       <c r="D9" s="30"/>
       <c r="E9" s="30"/>
       <c r="F9" s="30"/>
@@ -3327,37 +3207,37 @@
       <c r="J9" s="30"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D10" s="99"/>
-      <c r="E10" s="99"/>
-      <c r="F10" s="99"/>
-      <c r="G10" s="99"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D11" s="99"/>
-      <c r="E11" s="99"/>
-      <c r="F11" s="99"/>
-      <c r="G11" s="99"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D12" s="99"/>
-      <c r="E12" s="99"/>
-      <c r="F12" s="99"/>
-      <c r="G12" s="99"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D13" s="99"/>
-      <c r="E13" s="99"/>
-      <c r="F13" s="99"/>
-      <c r="G13" s="99"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="99"/>
-      <c r="E14" s="99"/>
-      <c r="F14" s="99"/>
-      <c r="G14" s="99"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -3437,6 +3317,7 @@
     <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3444,14 +3325,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100DB6EE-FC15-456B-9333-B04814A2904D}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
     <col min="3" max="3" width="9.44140625" customWidth="1"/>
     <col min="4" max="4" width="16.88671875" customWidth="1"/>
     <col min="6" max="6" width="15.5546875" customWidth="1"/>
@@ -3469,7 +3350,7 @@
     </row>
     <row r="4" spans="1:6" ht="22.8" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -3477,7 +3358,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>1</v>
@@ -3489,372 +3370,383 @@
         <v>3</v>
       </c>
       <c r="F5" s="24">
-        <v>45993</v>
+        <v>46024</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="63" t="s">
-        <v>130</v>
-      </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="64"/>
+      <c r="B6" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="61"/>
     </row>
     <row r="7" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="B7" s="65" t="s">
-        <v>151</v>
-      </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="66"/>
+        <v>150</v>
+      </c>
+      <c r="B7" s="75" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="76"/>
     </row>
     <row r="8" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="43" t="s">
-        <v>152</v>
-      </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="44"/>
+      <c r="B8" s="55" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="56"/>
     </row>
     <row r="9" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="43" t="s">
-        <v>153</v>
-      </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="44"/>
+      <c r="B9" s="55" t="s">
+        <v>148</v>
+      </c>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="56"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="44"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="56"/>
     </row>
     <row r="11" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="43" t="s">
-        <v>154</v>
-      </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="44"/>
+      <c r="B11" s="55" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="56"/>
     </row>
     <row r="12" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="44"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="56"/>
     </row>
     <row r="13" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13" s="43" t="s">
-        <v>91</v>
-      </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="44"/>
+        <v>89</v>
+      </c>
+      <c r="B13" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="56"/>
     </row>
     <row r="14" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B14" s="60" t="s">
-        <v>111</v>
-      </c>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="62"/>
+        <v>107</v>
+      </c>
+      <c r="B14" s="62" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="64"/>
     </row>
     <row r="15" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="B15" s="60" t="s">
-        <v>155</v>
-      </c>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="62"/>
+        <v>200</v>
+      </c>
+      <c r="B15" s="62" t="s">
+        <v>200</v>
+      </c>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="64"/>
     </row>
     <row r="16" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="B16" s="71" t="s">
+      <c r="A16" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="62" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="63"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="64"/>
+    </row>
+    <row r="17" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="B17" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="72"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="71" t="s">
-        <v>132</v>
-      </c>
-      <c r="F16" s="74"/>
-    </row>
-    <row r="17" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="B17" s="60" t="s">
-        <v>133</v>
-      </c>
-      <c r="C17" s="61"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="F17" s="62"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="F17" s="68"/>
     </row>
     <row r="18" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B18" s="60" t="s">
-        <v>135</v>
-      </c>
-      <c r="C18" s="61"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="F18" s="62"/>
+        <v>175</v>
+      </c>
+      <c r="B18" s="62" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" s="63"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="F18" s="44"/>
     </row>
     <row r="19" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B19" s="60" t="s">
-        <v>136</v>
-      </c>
-      <c r="C19" s="61"/>
-      <c r="D19" s="70"/>
-      <c r="E19" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="F19" s="62"/>
-    </row>
-    <row r="20" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+      <c r="B19" s="62" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="63"/>
+      <c r="D19" s="74"/>
+      <c r="E19" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="F19" s="44"/>
+    </row>
+    <row r="20" spans="1:10" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="B20" s="60" t="s">
-        <v>137</v>
-      </c>
-      <c r="C20" s="61"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="F20" s="62"/>
-    </row>
-    <row r="21" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+      <c r="B20" s="62" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="63"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="F20" s="44"/>
+    </row>
+    <row r="21" spans="1:10" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="B21" s="60" t="s">
-        <v>138</v>
-      </c>
-      <c r="C21" s="61"/>
-      <c r="D21" s="70"/>
-      <c r="E21" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="F21" s="62"/>
-    </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+      <c r="B21" s="62" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="63"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="F21" s="44"/>
+    </row>
+    <row r="22" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="B22" s="60" t="s">
-        <v>139</v>
-      </c>
-      <c r="C22" s="61"/>
-      <c r="D22" s="70"/>
-      <c r="E22" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="F22" s="62"/>
+        <v>179</v>
+      </c>
+      <c r="B22" s="62" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" s="63"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="F22" s="44"/>
     </row>
     <row r="23" spans="1:10" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="B23" s="60" t="s">
-        <v>140</v>
-      </c>
-      <c r="C23" s="61"/>
-      <c r="D23" s="70"/>
-      <c r="E23" s="60" t="s">
+        <v>180</v>
+      </c>
+      <c r="B23" s="62" t="s">
         <v>134</v>
       </c>
-      <c r="F23" s="62"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="F23" s="44"/>
     </row>
     <row r="24" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="B24" s="60" t="s">
-        <v>141</v>
-      </c>
-      <c r="C24" s="61"/>
-      <c r="D24" s="70"/>
-      <c r="E24" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="F24" s="62"/>
-      <c r="H24" s="99"/>
-      <c r="I24" s="99"/>
-      <c r="J24" s="99"/>
+        <v>181</v>
+      </c>
+      <c r="B24" s="62" t="s">
+        <v>135</v>
+      </c>
+      <c r="C24" s="63"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="F24" s="44"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="51"/>
     </row>
     <row r="25" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="B25" s="60" t="s">
-        <v>142</v>
-      </c>
-      <c r="C25" s="61"/>
-      <c r="D25" s="70"/>
-      <c r="E25" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="F25" s="62"/>
-      <c r="H25" s="99"/>
-      <c r="I25" s="99"/>
-      <c r="J25" s="99"/>
+        <v>182</v>
+      </c>
+      <c r="B25" s="62" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" s="63"/>
+      <c r="D25" s="74"/>
+      <c r="E25" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="F25" s="44"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="51"/>
     </row>
     <row r="26" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="B26" s="60" t="s">
-        <v>143</v>
-      </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="70"/>
-      <c r="E26" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="F26" s="62"/>
-      <c r="H26" s="99"/>
-      <c r="I26" s="99"/>
-      <c r="J26" s="99"/>
+        <v>183</v>
+      </c>
+      <c r="B26" s="62" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" s="63"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="F26" s="44"/>
+      <c r="H26" s="51"/>
+      <c r="I26" s="51"/>
+      <c r="J26" s="51"/>
     </row>
     <row r="27" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="B27" s="60" t="s">
-        <v>144</v>
-      </c>
-      <c r="C27" s="61"/>
-      <c r="D27" s="70"/>
-      <c r="E27" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="F27" s="62"/>
-      <c r="H27" s="99"/>
-      <c r="I27" s="99"/>
-      <c r="J27" s="99"/>
+        <v>184</v>
+      </c>
+      <c r="B27" s="62" t="s">
+        <v>138</v>
+      </c>
+      <c r="C27" s="63"/>
+      <c r="D27" s="74"/>
+      <c r="E27" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="F27" s="44"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="51"/>
     </row>
     <row r="28" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="B28" s="60" t="s">
-        <v>145</v>
-      </c>
-      <c r="C28" s="61"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="F28" s="62"/>
-      <c r="H28" s="99"/>
-      <c r="I28" s="99"/>
-      <c r="J28" s="99"/>
+        <v>185</v>
+      </c>
+      <c r="B28" s="62" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" s="63"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="F28" s="44"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="51"/>
     </row>
     <row r="29" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="B29" s="60" t="s">
-        <v>146</v>
-      </c>
-      <c r="C29" s="61"/>
-      <c r="D29" s="70"/>
-      <c r="E29" s="60" t="s">
-        <v>147</v>
-      </c>
-      <c r="F29" s="62"/>
+        <v>186</v>
+      </c>
+      <c r="B29" s="62" t="s">
+        <v>140</v>
+      </c>
+      <c r="C29" s="63"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="F29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="B30" s="60" t="s">
-        <v>148</v>
-      </c>
-      <c r="C30" s="61"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="F30" s="62"/>
-    </row>
-    <row r="31" spans="1:10" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="B31" s="67" t="s">
-        <v>149</v>
-      </c>
-      <c r="C31" s="68"/>
-      <c r="D31" s="69"/>
-      <c r="E31" s="67" t="s">
-        <v>134</v>
-      </c>
-      <c r="F31" s="79"/>
-    </row>
-    <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>187</v>
+      </c>
+      <c r="B30" s="62" t="s">
+        <v>141</v>
+      </c>
+      <c r="C30" s="63"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="62" t="s">
+        <v>142</v>
+      </c>
+      <c r="F30" s="64"/>
+    </row>
+    <row r="31" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B31" s="62" t="s">
+        <v>143</v>
+      </c>
+      <c r="C31" s="63"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="F31" s="44"/>
+    </row>
+    <row r="32" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B32" s="73" t="s">
+        <v>144</v>
+      </c>
+      <c r="C32" s="77"/>
+      <c r="D32" s="78"/>
+      <c r="E32" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="F32" s="46"/>
+    </row>
     <row r="34" spans="1:11" ht="22.8" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A34" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -3862,7 +3754,7 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C35" s="28" t="s">
         <v>1</v>
@@ -3874,287 +3766,284 @@
         <v>3</v>
       </c>
       <c r="F35" s="24">
-        <v>45993</v>
+        <v>46024</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="63" t="s">
-        <v>160</v>
-      </c>
-      <c r="C36" s="63"/>
-      <c r="D36" s="63"/>
-      <c r="E36" s="63"/>
-      <c r="F36" s="64"/>
+      <c r="B36" s="60" t="s">
+        <v>154</v>
+      </c>
+      <c r="C36" s="60"/>
+      <c r="D36" s="60"/>
+      <c r="E36" s="60"/>
+      <c r="F36" s="61"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="B37" s="58" t="s">
-        <v>151</v>
-      </c>
-      <c r="C37" s="58"/>
-      <c r="D37" s="58"/>
-      <c r="E37" s="58"/>
-      <c r="F37" s="59"/>
+        <v>145</v>
+      </c>
+      <c r="B37" s="87" t="s">
+        <v>146</v>
+      </c>
+      <c r="C37" s="87"/>
+      <c r="D37" s="87"/>
+      <c r="E37" s="87"/>
+      <c r="F37" s="88"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="48" t="s">
+      <c r="B38" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="48"/>
-      <c r="D38" s="48"/>
-      <c r="E38" s="48"/>
-      <c r="F38" s="49"/>
+      <c r="C38" s="89"/>
+      <c r="D38" s="89"/>
+      <c r="E38" s="89"/>
+      <c r="F38" s="90"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="48" t="s">
+      <c r="B39" s="89" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="49"/>
+      <c r="C39" s="89"/>
+      <c r="D39" s="89"/>
+      <c r="E39" s="89"/>
+      <c r="F39" s="90"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B40" s="48" t="s">
-        <v>161</v>
-      </c>
-      <c r="C40" s="48"/>
-      <c r="D40" s="48"/>
-      <c r="E40" s="48"/>
-      <c r="F40" s="49"/>
+      <c r="B40" s="89" t="s">
+        <v>155</v>
+      </c>
+      <c r="C40" s="89"/>
+      <c r="D40" s="89"/>
+      <c r="E40" s="89"/>
+      <c r="F40" s="90"/>
     </row>
     <row r="41" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="B41" s="75" t="s">
+        <v>126</v>
+      </c>
+      <c r="B41" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="76"/>
-      <c r="D41" s="77"/>
-      <c r="E41" s="75" t="s">
-        <v>132</v>
-      </c>
-      <c r="F41" s="78"/>
+      <c r="C41" s="70"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="69" t="s">
+        <v>127</v>
+      </c>
+      <c r="F41" s="72"/>
     </row>
     <row r="42" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="B42" s="50" t="s">
-        <v>163</v>
-      </c>
-      <c r="C42" s="52"/>
-      <c r="D42" s="53"/>
-      <c r="E42" s="50" t="s">
-        <v>134</v>
-      </c>
-      <c r="F42" s="51"/>
+        <v>156</v>
+      </c>
+      <c r="B42" s="83" t="s">
+        <v>157</v>
+      </c>
+      <c r="C42" s="85"/>
+      <c r="D42" s="86"/>
+      <c r="E42" s="83" t="s">
+        <v>129</v>
+      </c>
+      <c r="F42" s="84"/>
     </row>
     <row r="43" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B43" s="50" t="s">
-        <v>165</v>
-      </c>
-      <c r="C43" s="52"/>
-      <c r="D43" s="53"/>
-      <c r="E43" s="50" t="s">
-        <v>134</v>
-      </c>
-      <c r="F43" s="51"/>
+        <v>158</v>
+      </c>
+      <c r="B43" s="83" t="s">
+        <v>159</v>
+      </c>
+      <c r="C43" s="85"/>
+      <c r="D43" s="86"/>
+      <c r="E43" s="83" t="s">
+        <v>129</v>
+      </c>
+      <c r="F43" s="84"/>
     </row>
     <row r="44" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="B44" s="50" t="s">
-        <v>167</v>
-      </c>
-      <c r="C44" s="52"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="50" t="s">
-        <v>134</v>
-      </c>
-      <c r="F44" s="51"/>
-      <c r="H44" s="99"/>
-      <c r="I44" s="99"/>
-      <c r="J44" s="99"/>
-      <c r="K44" s="99"/>
+        <v>160</v>
+      </c>
+      <c r="B44" s="83" t="s">
+        <v>161</v>
+      </c>
+      <c r="C44" s="85"/>
+      <c r="D44" s="86"/>
+      <c r="E44" s="83" t="s">
+        <v>129</v>
+      </c>
+      <c r="F44" s="84"/>
+      <c r="H44" s="51"/>
+      <c r="I44" s="51"/>
+      <c r="J44" s="51"/>
+      <c r="K44" s="51"/>
     </row>
     <row r="45" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="B45" s="50" t="s">
-        <v>169</v>
-      </c>
-      <c r="C45" s="52"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="50" t="s">
-        <v>134</v>
-      </c>
-      <c r="F45" s="51"/>
-      <c r="H45" s="99"/>
-      <c r="I45" s="99"/>
-      <c r="J45" s="99"/>
-      <c r="K45" s="99"/>
+        <v>162</v>
+      </c>
+      <c r="B45" s="83" t="s">
+        <v>163</v>
+      </c>
+      <c r="C45" s="85"/>
+      <c r="D45" s="86"/>
+      <c r="E45" s="83" t="s">
+        <v>129</v>
+      </c>
+      <c r="F45" s="84"/>
+      <c r="H45" s="51"/>
+      <c r="I45" s="51"/>
+      <c r="J45" s="51"/>
+      <c r="K45" s="51"/>
     </row>
     <row r="46" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="B46" s="50" t="s">
-        <v>171</v>
-      </c>
-      <c r="C46" s="52"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="50" t="s">
-        <v>134</v>
-      </c>
-      <c r="F46" s="51"/>
-      <c r="H46" s="99"/>
-      <c r="I46" s="99"/>
-      <c r="J46" s="99"/>
-      <c r="K46" s="99"/>
+        <v>164</v>
+      </c>
+      <c r="B46" s="83" t="s">
+        <v>165</v>
+      </c>
+      <c r="C46" s="85"/>
+      <c r="D46" s="86"/>
+      <c r="E46" s="83" t="s">
+        <v>129</v>
+      </c>
+      <c r="F46" s="84"/>
+      <c r="H46" s="51"/>
+      <c r="I46" s="51"/>
+      <c r="J46" s="51"/>
+      <c r="K46" s="51"/>
     </row>
     <row r="47" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B47" s="50" t="s">
-        <v>173</v>
-      </c>
-      <c r="C47" s="52"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="50" t="s">
-        <v>134</v>
-      </c>
-      <c r="F47" s="51"/>
-      <c r="H47" s="99"/>
-      <c r="I47" s="99"/>
-      <c r="J47" s="99"/>
-      <c r="K47" s="99"/>
+        <v>166</v>
+      </c>
+      <c r="B47" s="83" t="s">
+        <v>167</v>
+      </c>
+      <c r="C47" s="85"/>
+      <c r="D47" s="86"/>
+      <c r="E47" s="83" t="s">
+        <v>129</v>
+      </c>
+      <c r="F47" s="84"/>
+      <c r="H47" s="51"/>
+      <c r="I47" s="51"/>
+      <c r="J47" s="51"/>
+      <c r="K47" s="51"/>
     </row>
     <row r="48" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="B48" s="50" t="s">
-        <v>175</v>
-      </c>
-      <c r="C48" s="52"/>
-      <c r="D48" s="53"/>
-      <c r="E48" s="50" t="s">
-        <v>134</v>
-      </c>
-      <c r="F48" s="51"/>
-      <c r="H48" s="99"/>
-      <c r="I48" s="99"/>
-      <c r="J48" s="99"/>
-      <c r="K48" s="99"/>
+        <v>168</v>
+      </c>
+      <c r="B48" s="83" t="s">
+        <v>169</v>
+      </c>
+      <c r="C48" s="85"/>
+      <c r="D48" s="86"/>
+      <c r="E48" s="83" t="s">
+        <v>129</v>
+      </c>
+      <c r="F48" s="84"/>
+      <c r="H48" s="51"/>
+      <c r="I48" s="51"/>
+      <c r="J48" s="51"/>
+      <c r="K48" s="51"/>
     </row>
     <row r="49" spans="1:11" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="B49" s="50" t="s">
-        <v>198</v>
-      </c>
-      <c r="C49" s="52"/>
-      <c r="D49" s="53"/>
-      <c r="E49" s="50" t="s">
-        <v>199</v>
-      </c>
-      <c r="F49" s="51"/>
-      <c r="H49" s="99"/>
-      <c r="I49" s="99"/>
-      <c r="J49" s="99"/>
-      <c r="K49" s="99"/>
+        <v>191</v>
+      </c>
+      <c r="B49" s="83" t="s">
+        <v>192</v>
+      </c>
+      <c r="C49" s="85"/>
+      <c r="D49" s="86"/>
+      <c r="E49" s="83" t="s">
+        <v>193</v>
+      </c>
+      <c r="F49" s="84"/>
+      <c r="H49" s="51"/>
+      <c r="I49" s="51"/>
+      <c r="J49" s="51"/>
+      <c r="K49" s="51"/>
     </row>
     <row r="50" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="B50" s="50" t="s">
-        <v>202</v>
-      </c>
-      <c r="C50" s="52"/>
-      <c r="D50" s="53"/>
-      <c r="E50" s="50" t="s">
-        <v>199</v>
-      </c>
-      <c r="F50" s="51"/>
-      <c r="H50" s="99"/>
-      <c r="I50" s="99"/>
-      <c r="J50" s="99"/>
-      <c r="K50" s="99"/>
+        <v>194</v>
+      </c>
+      <c r="B50" s="83" t="s">
+        <v>196</v>
+      </c>
+      <c r="C50" s="85"/>
+      <c r="D50" s="86"/>
+      <c r="E50" s="83" t="s">
+        <v>193</v>
+      </c>
+      <c r="F50" s="84"/>
+      <c r="H50" s="51"/>
+      <c r="I50" s="51"/>
+      <c r="J50" s="51"/>
+      <c r="K50" s="51"/>
     </row>
     <row r="51" spans="1:11" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="B51" s="54" t="s">
-        <v>203</v>
-      </c>
-      <c r="C51" s="55"/>
-      <c r="D51" s="56"/>
-      <c r="E51" s="54" t="s">
-        <v>199</v>
-      </c>
-      <c r="F51" s="57"/>
-      <c r="H51" s="99"/>
-      <c r="I51" s="99"/>
-      <c r="J51" s="99"/>
-      <c r="K51" s="99"/>
+        <v>195</v>
+      </c>
+      <c r="B51" s="79" t="s">
+        <v>197</v>
+      </c>
+      <c r="C51" s="80"/>
+      <c r="D51" s="81"/>
+      <c r="E51" s="79" t="s">
+        <v>193</v>
+      </c>
+      <c r="F51" s="82"/>
+      <c r="H51" s="51"/>
+      <c r="I51" s="51"/>
+      <c r="J51" s="51"/>
+      <c r="K51" s="51"/>
     </row>
     <row r="52" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="69">
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
+  <mergeCells count="56">
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="E49:F49"/>
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="B36:F36"/>
     <mergeCell ref="B7:F7"/>
@@ -4164,37 +4053,27 @@
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B17:D17"/>
     <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B13:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>